<commit_message>
XP calculator+ Work on Spawn
Spawn x tiles
</commit_message>
<xml_diff>
--- a/Game Design/BL_Map_Tiles.xlsx
+++ b/Game Design/BL_Map_Tiles.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="49665" yWindow="75" windowWidth="16860" windowHeight="6255" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="terrain" sheetId="1" r:id="rId1"/>
+    <sheet name="tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="level up" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'level up'!$A$1:$H$6</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="70">
   <si>
     <t>Temperature</t>
   </si>
@@ -130,9 +133,6 @@
   </si>
   <si>
     <t>Ice Lion</t>
-  </si>
-  <si>
-    <t>Red Lion</t>
   </si>
   <si>
     <t>Green Lion</t>
@@ -215,6 +215,60 @@
   </si>
   <si>
     <t>difficulty level</t>
+  </si>
+  <si>
+    <t>lvl</t>
+  </si>
+  <si>
+    <t>enemy</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>aw</t>
+  </si>
+  <si>
+    <t>Horned Lion</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>level up system</t>
+  </si>
+  <si>
+    <t>fb collect n spend resources</t>
+  </si>
+  <si>
+    <t>fb starvation</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Def</t>
+  </si>
+  <si>
+    <t>Glory</t>
+  </si>
+  <si>
+    <t>Gl step</t>
   </si>
 </sst>
 </file>
@@ -261,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +411,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -797,7 +875,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -859,15 +937,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="15" xfId="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -876,6 +948,83 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="15" borderId="13" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="15" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="15" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="15" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="15" borderId="32" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="20" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="18" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="19" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="20" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -898,53 +1047,6 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="15" borderId="13" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="15" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="15" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="15" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="15" borderId="32" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
@@ -1249,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,50 +1368,50 @@
     <col min="19" max="19" width="4.7109375" customWidth="1"/>
     <col min="20" max="20" width="9.140625" style="26"/>
     <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="51" t="s">
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="51" t="s">
+      <c r="E1" s="77"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="52"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="H1" s="77"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="N1" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="57" t="s">
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="61"/>
+      <c r="S1" s="52"/>
       <c r="T1" s="1"/>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1339,7 +1441,7 @@
       <c r="I2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="54"/>
+      <c r="J2" s="79"/>
       <c r="N2" s="39" t="s">
         <v>25</v>
       </c>
@@ -1352,13 +1454,13 @@
       <c r="Q2" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="58" t="s">
+      <c r="R2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="61"/>
+      <c r="S2" s="52"/>
       <c r="T2" s="1"/>
       <c r="V2" s="39" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="W2" s="39" t="s">
         <v>35</v>
@@ -1370,7 +1472,7 @@
         <v>37</v>
       </c>
       <c r="Z2" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
@@ -1398,23 +1500,23 @@
       <c r="M3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="40">
-        <v>0.05</v>
-      </c>
-      <c r="O3" s="40">
-        <v>0</v>
-      </c>
-      <c r="P3" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="43">
-        <v>0.15</v>
-      </c>
-      <c r="R3" s="59">
+      <c r="N3" s="64">
+        <v>0.04</v>
+      </c>
+      <c r="O3" s="65">
+        <v>0</v>
+      </c>
+      <c r="P3" s="66">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="67">
+        <v>0.1</v>
+      </c>
+      <c r="R3" s="50">
         <f t="shared" ref="R3:R14" si="0">SUM(N3:Q3)</f>
-        <v>0.2</v>
-      </c>
-      <c r="S3" s="62"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S3" s="53"/>
       <c r="T3" s="1">
         <v>1</v>
       </c>
@@ -1430,7 +1532,7 @@
       <c r="X3" s="40">
         <v>0</v>
       </c>
-      <c r="Y3" s="67">
+      <c r="Y3" s="58">
         <v>0.15</v>
       </c>
       <c r="Z3" s="40">
@@ -1462,23 +1564,23 @@
       <c r="M4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="40">
+      <c r="N4" s="64">
+        <v>0.04</v>
+      </c>
+      <c r="O4" s="65">
+        <v>0.08</v>
+      </c>
+      <c r="P4" s="66">
+        <v>0.15</v>
+      </c>
+      <c r="Q4" s="67">
         <v>0.05</v>
       </c>
-      <c r="O4" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="P4" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="Q4" s="43">
-        <v>0.05</v>
-      </c>
-      <c r="R4" s="59">
+      <c r="R4" s="50">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="S4" s="62"/>
+        <v>0.32</v>
+      </c>
+      <c r="S4" s="53"/>
       <c r="T4" s="1">
         <v>2</v>
       </c>
@@ -1488,13 +1590,13 @@
       <c r="V4" s="40">
         <v>0</v>
       </c>
-      <c r="W4" s="67">
+      <c r="W4" s="58">
         <v>0.1</v>
       </c>
       <c r="X4" s="40">
         <v>0</v>
       </c>
-      <c r="Y4" s="67">
+      <c r="Y4" s="58">
         <v>0.1</v>
       </c>
       <c r="Z4" s="40">
@@ -1526,23 +1628,23 @@
       <c r="M5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="O5" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="P5" s="40">
-        <v>0.05</v>
-      </c>
-      <c r="Q5" s="43">
-        <v>0.05</v>
-      </c>
-      <c r="R5" s="59">
+      <c r="N5" s="64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O5" s="65">
+        <v>0.08</v>
+      </c>
+      <c r="P5" s="66">
+        <v>0.04</v>
+      </c>
+      <c r="Q5" s="67">
+        <v>0.04</v>
+      </c>
+      <c r="R5" s="50">
         <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="S5" s="62"/>
+        <v>0.23000000000000004</v>
+      </c>
+      <c r="S5" s="53"/>
       <c r="T5" s="1">
         <v>3</v>
       </c>
@@ -1558,7 +1660,7 @@
       <c r="X5" s="40">
         <v>0</v>
       </c>
-      <c r="Y5" s="67">
+      <c r="Y5" s="58">
         <v>0.15</v>
       </c>
       <c r="Z5" s="40">
@@ -1590,36 +1692,36 @@
       <c r="M6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="O6" s="40">
-        <v>0.15</v>
-      </c>
-      <c r="P6" s="40">
+      <c r="N6" s="64">
+        <v>0.1</v>
+      </c>
+      <c r="O6" s="65">
+        <v>0.08</v>
+      </c>
+      <c r="P6" s="66">
+        <v>0.04</v>
+      </c>
+      <c r="Q6" s="67">
         <v>0.05</v>
       </c>
-      <c r="Q6" s="43">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="R6" s="59">
+      <c r="R6" s="50">
         <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-      <c r="S6" s="62"/>
+        <v>0.27</v>
+      </c>
+      <c r="S6" s="53"/>
       <c r="T6" s="1">
         <v>4</v>
       </c>
       <c r="U6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="67">
+      <c r="V6" s="58">
         <v>0.1</v>
       </c>
       <c r="W6" s="40">
         <v>0</v>
       </c>
-      <c r="X6" s="67">
+      <c r="X6" s="58">
         <v>0.05</v>
       </c>
       <c r="Y6" s="40">
@@ -1654,36 +1756,36 @@
       <c r="M7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="40">
-        <v>0.15</v>
-      </c>
-      <c r="O7" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="P7" s="40">
+      <c r="N7" s="64">
+        <v>0.1</v>
+      </c>
+      <c r="O7" s="65">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="66">
+        <v>0.04</v>
+      </c>
+      <c r="Q7" s="67">
         <v>0.05</v>
       </c>
-      <c r="Q7" s="43">
-        <v>0.05</v>
-      </c>
-      <c r="R7" s="59">
+      <c r="R7" s="50">
         <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="S7" s="62"/>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="S7" s="53"/>
       <c r="T7" s="1">
         <v>5</v>
       </c>
       <c r="U7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="67">
+      <c r="V7" s="58">
         <v>0.1</v>
       </c>
       <c r="W7" s="40">
         <v>0</v>
       </c>
-      <c r="X7" s="67">
+      <c r="X7" s="58">
         <v>0.05</v>
       </c>
       <c r="Y7" s="40">
@@ -1718,33 +1820,33 @@
       <c r="M8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="O8" s="40">
+      <c r="N8" s="64">
+        <v>0.08</v>
+      </c>
+      <c r="O8" s="65">
         <v>0.05</v>
       </c>
-      <c r="P8" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="Q8" s="43">
+      <c r="P8" s="66">
+        <v>0.15</v>
+      </c>
+      <c r="Q8" s="67">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="R8" s="59">
+      <c r="R8" s="50">
         <f t="shared" si="0"/>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="S8" s="62"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="S8" s="53"/>
       <c r="T8" s="1">
         <v>6</v>
       </c>
       <c r="U8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="V8" s="67">
+      <c r="V8" s="58">
         <v>0.1</v>
       </c>
-      <c r="W8" s="67">
+      <c r="W8" s="58">
         <v>0.1</v>
       </c>
       <c r="X8" s="40">
@@ -1782,30 +1884,30 @@
       <c r="M9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="40">
-        <v>0.43</v>
-      </c>
-      <c r="O9" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="P9" s="40">
+      <c r="N9" s="64">
+        <v>0.2</v>
+      </c>
+      <c r="O9" s="65">
         <v>0.05</v>
       </c>
-      <c r="Q9" s="43">
-        <v>0</v>
-      </c>
-      <c r="R9" s="59">
+      <c r="P9" s="66">
+        <v>0.03</v>
+      </c>
+      <c r="Q9" s="67">
+        <v>0</v>
+      </c>
+      <c r="R9" s="50">
         <f t="shared" si="0"/>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="S9" s="62"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S9" s="53"/>
       <c r="T9" s="1">
         <v>7</v>
       </c>
       <c r="U9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="V9" s="67">
+      <c r="V9" s="58">
         <v>0.05</v>
       </c>
       <c r="W9" s="40">
@@ -1817,7 +1919,7 @@
       <c r="Y9" s="40">
         <v>0</v>
       </c>
-      <c r="Z9" s="67">
+      <c r="Z9" s="58">
         <v>0.1</v>
       </c>
     </row>
@@ -1846,23 +1948,23 @@
       <c r="M10" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="40">
-        <v>0.33</v>
-      </c>
-      <c r="O10" s="40">
-        <v>0.3</v>
-      </c>
-      <c r="P10" s="40">
-        <v>0.05</v>
-      </c>
-      <c r="Q10" s="43">
-        <v>0</v>
-      </c>
-      <c r="R10" s="59">
+      <c r="N10" s="64">
+        <v>0.18</v>
+      </c>
+      <c r="O10" s="65">
+        <v>0.22</v>
+      </c>
+      <c r="P10" s="66">
+        <v>0.04</v>
+      </c>
+      <c r="Q10" s="67">
+        <v>0</v>
+      </c>
+      <c r="R10" s="50">
         <f t="shared" si="0"/>
-        <v>0.68</v>
-      </c>
-      <c r="S10" s="62"/>
+        <v>0.44</v>
+      </c>
+      <c r="S10" s="53"/>
       <c r="T10" s="1">
         <v>8</v>
       </c>
@@ -1881,7 +1983,7 @@
       <c r="Y10" s="40">
         <v>0</v>
       </c>
-      <c r="Z10" s="67">
+      <c r="Z10" s="58">
         <v>0.1</v>
       </c>
     </row>
@@ -1910,23 +2012,23 @@
       <c r="M11" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="N11" s="40">
-        <v>0.33</v>
-      </c>
-      <c r="O11" s="40">
-        <v>0.25</v>
-      </c>
-      <c r="P11" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="Q11" s="43">
-        <v>0</v>
-      </c>
-      <c r="R11" s="59">
+      <c r="N11" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="O11" s="65">
+        <v>0.18</v>
+      </c>
+      <c r="P11" s="66">
+        <v>0.15</v>
+      </c>
+      <c r="Q11" s="67">
+        <v>0</v>
+      </c>
+      <c r="R11" s="50">
         <f t="shared" si="0"/>
-        <v>0.78</v>
-      </c>
-      <c r="S11" s="62"/>
+        <v>0.48</v>
+      </c>
+      <c r="S11" s="53"/>
       <c r="T11" s="1">
         <v>9</v>
       </c>
@@ -1936,7 +2038,7 @@
       <c r="V11" s="40">
         <v>0</v>
       </c>
-      <c r="W11" s="67">
+      <c r="W11" s="58">
         <v>0.1</v>
       </c>
       <c r="X11" s="40">
@@ -1945,7 +2047,7 @@
       <c r="Y11" s="40">
         <v>0</v>
       </c>
-      <c r="Z11" s="67">
+      <c r="Z11" s="58">
         <v>0.1</v>
       </c>
     </row>
@@ -1974,23 +2076,23 @@
       <c r="M12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="40">
-        <v>0.05</v>
-      </c>
-      <c r="O12" s="40">
-        <v>0</v>
-      </c>
-      <c r="P12" s="40">
-        <v>0.05</v>
-      </c>
-      <c r="Q12" s="43">
-        <v>0.13</v>
-      </c>
-      <c r="R12" s="59">
+      <c r="N12" s="64">
+        <v>0.04</v>
+      </c>
+      <c r="O12" s="65">
+        <v>0</v>
+      </c>
+      <c r="P12" s="66">
+        <v>0.03</v>
+      </c>
+      <c r="Q12" s="67">
+        <v>0.1</v>
+      </c>
+      <c r="R12" s="50">
         <f t="shared" si="0"/>
-        <v>0.23</v>
-      </c>
-      <c r="S12" s="62"/>
+        <v>0.17</v>
+      </c>
+      <c r="S12" s="53"/>
       <c r="T12" s="1">
         <v>10</v>
       </c>
@@ -2003,7 +2105,7 @@
       <c r="W12" s="40">
         <v>0</v>
       </c>
-      <c r="X12" s="67">
+      <c r="X12" s="58">
         <v>0.15</v>
       </c>
       <c r="Y12" s="40">
@@ -2038,36 +2140,36 @@
       <c r="M13" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="40">
+      <c r="N13" s="64">
         <v>0.05</v>
       </c>
-      <c r="O13" s="40">
+      <c r="O13" s="65">
         <v>0.05</v>
       </c>
-      <c r="P13" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="Q13" s="43">
-        <v>0.13</v>
-      </c>
-      <c r="R13" s="59">
+      <c r="P13" s="66">
+        <v>0.15</v>
+      </c>
+      <c r="Q13" s="67">
+        <v>0.1</v>
+      </c>
+      <c r="R13" s="50">
         <f t="shared" si="0"/>
-        <v>0.43000000000000005</v>
-      </c>
-      <c r="S13" s="62"/>
+        <v>0.35</v>
+      </c>
+      <c r="S13" s="53"/>
       <c r="T13" s="1">
         <v>11</v>
       </c>
       <c r="U13" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="V13" s="67">
+      <c r="V13" s="58">
         <v>0.05</v>
       </c>
-      <c r="W13" s="67">
+      <c r="W13" s="58">
         <v>0.1</v>
       </c>
-      <c r="X13" s="67">
+      <c r="X13" s="58">
         <v>0.15</v>
       </c>
       <c r="Y13" s="40">
@@ -2102,42 +2204,42 @@
       <c r="M14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="44">
-        <v>0.25</v>
-      </c>
-      <c r="O14" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="P14" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="45">
-        <v>0.05</v>
-      </c>
-      <c r="R14" s="60">
+      <c r="N14" s="68">
+        <v>0.18</v>
+      </c>
+      <c r="O14" s="69">
+        <v>0.18</v>
+      </c>
+      <c r="P14" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="71">
+        <v>0</v>
+      </c>
+      <c r="R14" s="51">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="S14" s="62"/>
+        <v>0.36</v>
+      </c>
+      <c r="S14" s="53"/>
       <c r="T14" s="1">
         <v>12</v>
       </c>
       <c r="U14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="V14" s="44">
-        <v>0</v>
-      </c>
-      <c r="W14" s="44">
-        <v>0</v>
-      </c>
-      <c r="X14" s="44">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="44">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="68">
+      <c r="V14" s="72">
+        <v>0.05</v>
+      </c>
+      <c r="W14" s="43">
+        <v>0</v>
+      </c>
+      <c r="X14" s="43">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="43">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="59">
         <v>0.1</v>
       </c>
     </row>
@@ -2160,41 +2262,41 @@
       <c r="J15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="46">
+      <c r="N15" s="44">
         <f>SUM(N3:N14)</f>
-        <v>2.0900000000000003</v>
-      </c>
-      <c r="O15" s="47">
+        <v>1.23</v>
+      </c>
+      <c r="O15" s="45">
         <f>SUM(O3:O14)</f>
-        <v>1.5</v>
-      </c>
-      <c r="P15" s="47">
+        <v>1.0699999999999998</v>
+      </c>
+      <c r="P15" s="45">
         <f>SUM(P3:P14)</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q15" s="48">
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="Q15" s="46">
         <f>SUM(Q3:Q14)</f>
-        <v>0.75000000000000011</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="R15" s="41"/>
       <c r="S15" s="41"/>
-      <c r="V15" s="69">
+      <c r="V15" s="60">
         <f>SUM(V3:V14)</f>
-        <v>0.4</v>
-      </c>
-      <c r="W15" s="70">
+        <v>0.45</v>
+      </c>
+      <c r="W15" s="61">
         <f>SUM(W3:W14)</f>
         <v>0.4</v>
       </c>
-      <c r="X15" s="70">
+      <c r="X15" s="61">
         <f>SUM(X3:X14)</f>
         <v>0.4</v>
       </c>
-      <c r="Y15" s="70">
+      <c r="Y15" s="61">
         <f>SUM(Y3:Y14)</f>
         <v>0.4</v>
       </c>
-      <c r="Z15" s="71">
+      <c r="Z15" s="62">
         <f>SUM(Z3:Z14)</f>
         <v>0.4</v>
       </c>
@@ -2217,6 +2319,9 @@
       <c r="I16" s="8"/>
       <c r="J16" s="22" t="s">
         <v>24</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -2238,22 +2343,22 @@
       <c r="J17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="64" t="s">
+      <c r="M17" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="N17" s="65">
+      <c r="N17" s="56">
         <v>7</v>
       </c>
-      <c r="O17" s="65">
+      <c r="O17" s="56">
         <v>14</v>
       </c>
-      <c r="P17" s="65">
+      <c r="P17" s="56">
         <v>14</v>
       </c>
-      <c r="Q17" s="66">
+      <c r="Q17" s="57">
         <v>28</v>
       </c>
-      <c r="U17" s="56" t="s">
+      <c r="U17" s="47" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2277,18 +2382,18 @@
         <v>23</v>
       </c>
       <c r="M18" t="s">
-        <v>51</v>
-      </c>
-      <c r="N18" s="63">
+        <v>50</v>
+      </c>
+      <c r="N18" s="54">
         <v>4</v>
       </c>
-      <c r="O18" s="63">
+      <c r="O18" s="54">
         <v>1</v>
       </c>
-      <c r="P18" s="63">
+      <c r="P18" s="54">
         <v>1</v>
       </c>
-      <c r="Q18" s="63">
+      <c r="Q18" s="54">
         <v>1</v>
       </c>
     </row>
@@ -2314,7 +2419,7 @@
       <c r="M19" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="63">
+      <c r="N19" s="54">
         <v>2</v>
       </c>
     </row>
@@ -2558,10 +2663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F25"/>
+  <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,43 +2680,45 @@
   <sheetData>
     <row r="1" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="72"/>
+      <c r="C2" s="63"/>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="3:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="72"/>
+      <c r="C4" s="73" t="s">
+        <v>59</v>
+      </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="3:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="72"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="7"/>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="3:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="72"/>
+      <c r="D8" s="63"/>
       <c r="F8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="72"/>
+      <c r="D10" s="63"/>
       <c r="F10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="3:6" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="72"/>
+      <c r="D12" s="63"/>
       <c r="F12" t="s">
         <v>2</v>
       </c>
@@ -2619,62 +2726,77 @@
     <row r="13" spans="3:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="72"/>
+        <v>42</v>
+      </c>
+      <c r="D14" s="63"/>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="3:6" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="72"/>
+      <c r="D16" s="63"/>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="72"/>
+      <c r="E17" s="63"/>
       <c r="F17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="63"/>
+      <c r="F18" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="72"/>
-      <c r="F18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="72"/>
+        <v>42</v>
+      </c>
+      <c r="C20" s="63"/>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="72"/>
+      <c r="D22" s="63"/>
       <c r="F22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="63"/>
+      <c r="F23" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="72"/>
-      <c r="F23" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="72"/>
+      <c r="C25" s="63"/>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2684,12 +2806,195 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26">
+        <v>0</v>
+      </c>
+      <c r="C2" s="26">
+        <f>B3-B2</f>
+        <v>100</v>
+      </c>
+      <c r="D2" s="26">
+        <v>20</v>
+      </c>
+      <c r="E2" s="26">
+        <v>6</v>
+      </c>
+      <c r="F2" s="26">
+        <v>2</v>
+      </c>
+      <c r="G2" s="26">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26">
+        <v>100</v>
+      </c>
+      <c r="C3" s="26">
+        <f t="shared" ref="C3:C5" si="0">B4-B3</f>
+        <v>400</v>
+      </c>
+      <c r="D3" s="26">
+        <v>25</v>
+      </c>
+      <c r="E3" s="26">
+        <v>9</v>
+      </c>
+      <c r="F3" s="26">
+        <v>4</v>
+      </c>
+      <c r="G3" s="26">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26">
+        <v>500</v>
+      </c>
+      <c r="C4" s="26">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="D4" s="26">
+        <v>30</v>
+      </c>
+      <c r="E4" s="26">
+        <v>11</v>
+      </c>
+      <c r="F4" s="26">
+        <v>6</v>
+      </c>
+      <c r="G4" s="26">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26">
+        <v>1300</v>
+      </c>
+      <c r="C5" s="26">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="D5" s="26">
+        <v>35</v>
+      </c>
+      <c r="E5" s="26">
+        <v>14</v>
+      </c>
+      <c r="F5" s="26">
+        <v>8</v>
+      </c>
+      <c r="G5" s="26">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="K5" s="26">
+        <v>50</v>
+      </c>
+      <c r="L5" s="26">
+        <v>100</v>
+      </c>
+      <c r="M5" s="26">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>5</v>
+      </c>
+      <c r="B6" s="26">
+        <v>2500</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26">
+        <v>40</v>
+      </c>
+      <c r="E6" s="26">
+        <v>17</v>
+      </c>
+      <c r="F6" s="26">
+        <v>10</v>
+      </c>
+      <c r="G6" s="26">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
spawning 15 opponents 15 different stat sets for the opponents
</commit_message>
<xml_diff>
--- a/Game Design/BL_Map_Tiles.xlsx
+++ b/Game Design/BL_Map_Tiles.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="49665" yWindow="75" windowWidth="16860" windowHeight="6255" activeTab="2"/>
+    <workbookView xWindow="49665" yWindow="75" windowWidth="16860" windowHeight="6255" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="terrain" sheetId="1" r:id="rId1"/>
     <sheet name="tasks" sheetId="2" r:id="rId2"/>
     <sheet name="level up" sheetId="3" r:id="rId3"/>
+    <sheet name="MonsterSpawn" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'level up'!$A$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MonsterSpawn!$A$19:$M$34</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="123">
   <si>
     <t>Temperature</t>
   </si>
@@ -269,6 +271,165 @@
   </si>
   <si>
     <t>Gl step</t>
+  </si>
+  <si>
+    <t>Monsters</t>
+  </si>
+  <si>
+    <t>DesertLion</t>
+  </si>
+  <si>
+    <t>GreenLion</t>
+  </si>
+  <si>
+    <t>HornedLion</t>
+  </si>
+  <si>
+    <t>IceLion</t>
+  </si>
+  <si>
+    <t>SilverLion</t>
+  </si>
+  <si>
+    <t>TigerLion</t>
+  </si>
+  <si>
+    <t>DesertJackal</t>
+  </si>
+  <si>
+    <t>GreenJackal</t>
+  </si>
+  <si>
+    <t>IceJackal</t>
+  </si>
+  <si>
+    <t>SilverJackal</t>
+  </si>
+  <si>
+    <t>DesertMammoth</t>
+  </si>
+  <si>
+    <t>GreenMammoth</t>
+  </si>
+  <si>
+    <t>IceMammoth</t>
+  </si>
+  <si>
+    <t>MammothParent</t>
+  </si>
+  <si>
+    <t>SilverMammoth</t>
+  </si>
+  <si>
+    <t>Primary Tile</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Texture</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>dmg</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>att</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>glory</t>
+  </si>
+  <si>
+    <t>sp. Att 1</t>
+  </si>
+  <si>
+    <t>sp. Att 2</t>
+  </si>
+  <si>
+    <t>Desert&amp;Savannah</t>
+  </si>
+  <si>
+    <t>debuffing attack</t>
+  </si>
+  <si>
+    <t>Lion Pride (buff strength)</t>
+  </si>
+  <si>
+    <t>Jungle</t>
+  </si>
+  <si>
+    <t>Poisoning attack ( extended damage)</t>
+  </si>
+  <si>
+    <t>Grassland&amp;Forest</t>
+  </si>
+  <si>
+    <t>double damage attack</t>
+  </si>
+  <si>
+    <t>Arctic</t>
+  </si>
+  <si>
+    <t>freeze (paralizing attack)</t>
+  </si>
+  <si>
+    <t>Savannah</t>
+  </si>
+  <si>
+    <t>Eye for an Eye (reflects damage)</t>
+  </si>
+  <si>
+    <t>Jungle&amp;Savannah</t>
+  </si>
+  <si>
+    <t>Jackal</t>
+  </si>
+  <si>
+    <t>Steal life (takes HP from player)</t>
+  </si>
+  <si>
+    <t>healing wind (heal self)</t>
+  </si>
+  <si>
+    <t>strength of the Jungle(armor buff)</t>
+  </si>
+  <si>
+    <t>Artic&amp;Forest</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Forest (all)</t>
+  </si>
+  <si>
+    <t>Mammoth</t>
+  </si>
+  <si>
+    <t>doubedamage attack</t>
+  </si>
+  <si>
+    <t>Posoning Trunk (dmg 3 rounds)</t>
+  </si>
+  <si>
+    <t>Grassland</t>
+  </si>
+  <si>
+    <t>Trample (doubledamage)</t>
+  </si>
+  <si>
+    <t>MUSTER</t>
   </si>
 </sst>
 </file>
@@ -315,7 +476,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,8 +596,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -870,12 +1055,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1046,6 +1310,75 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="16" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="16" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1352,7 +1685,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="L1" sqref="L1:R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,7 +3141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2997,4 +3330,1865 @@
   <autoFilter ref="A1:H6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="26"/>
+      <c r="C1" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="110"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="C2" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="84" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="110"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="L3" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="M3" s="102"/>
+      <c r="N3" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="50">
+        <f>SUM(C3:Q3)</f>
+        <v>0.2</v>
+      </c>
+      <c r="S3" s="110"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="L4" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="M4" s="102"/>
+      <c r="N4" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="O4" s="102"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="50">
+        <f t="shared" ref="R4:R14" si="0">SUM(C4:Q4)</f>
+        <v>0.2</v>
+      </c>
+      <c r="S4" s="110"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="L5" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="102"/>
+      <c r="N5" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="O5" s="102"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="50">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="S5" s="110"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="R6" s="50">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="S6" s="110"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="N7" s="102"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="102"/>
+      <c r="Q7" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="R7" s="50">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="S7" s="110"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="M8" s="102"/>
+      <c r="N8" s="102"/>
+      <c r="O8" s="102"/>
+      <c r="P8" s="102"/>
+      <c r="Q8" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="R8" s="50">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="S8" s="110"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
+      <c r="O9" s="102"/>
+      <c r="P9" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="Q9" s="102"/>
+      <c r="R9" s="50">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="S9" s="110"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="N10" s="102"/>
+      <c r="O10" s="102"/>
+      <c r="P10" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="50">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="S10" s="110"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="K11" s="102"/>
+      <c r="L11" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="M11" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="N11" s="102"/>
+      <c r="O11" s="102"/>
+      <c r="P11" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="50">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="S11" s="110"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="100"/>
+      <c r="E12" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="R12" s="50">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="S12" s="110"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="H13" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="R13" s="50">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="S13" s="110"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="104"/>
+      <c r="D14" s="105">
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="104"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="107">
+        <v>0.05</v>
+      </c>
+      <c r="I14" s="107">
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="106"/>
+      <c r="K14" s="106"/>
+      <c r="L14" s="106"/>
+      <c r="M14" s="106"/>
+      <c r="N14" s="106"/>
+      <c r="O14" s="107">
+        <v>0.05</v>
+      </c>
+      <c r="P14" s="106"/>
+      <c r="Q14" s="106"/>
+      <c r="R14" s="50">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="S14" s="110"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26"/>
+      <c r="C15" s="44">
+        <f>SUM(C3:C14)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="45">
+        <f>SUM(D3:D14)</f>
+        <v>0.05</v>
+      </c>
+      <c r="E15" s="45">
+        <f>SUM(E3:E14)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="46">
+        <f>SUM(F3:F14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="G15" s="46">
+        <f>SUM(G3:G14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H15" s="46">
+        <f>SUM(H3:H14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="I15" s="46">
+        <f>SUM(I3:I14)</f>
+        <v>0.05</v>
+      </c>
+      <c r="J15" s="46">
+        <f>SUM(J3:J14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="K15" s="46">
+        <f>SUM(K3:K14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="L15" s="46">
+        <f>SUM(L3:L14)</f>
+        <v>0.25</v>
+      </c>
+      <c r="M15" s="46">
+        <f>SUM(M3:M14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N15" s="46">
+        <f>SUM(N3:N14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="O15" s="46">
+        <f>SUM(O3:O14)</f>
+        <v>0.05</v>
+      </c>
+      <c r="P15" s="46">
+        <f>SUM(P3:P14)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="Q15" s="46">
+        <f>SUM(Q3:Q14)</f>
+        <v>0.25</v>
+      </c>
+      <c r="R15" s="41"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
+      <c r="B17" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="56">
+        <v>10</v>
+      </c>
+      <c r="D17" s="56">
+        <v>10</v>
+      </c>
+      <c r="E17" s="56">
+        <v>10</v>
+      </c>
+      <c r="F17" s="56">
+        <v>15</v>
+      </c>
+      <c r="G17" s="56">
+        <v>20</v>
+      </c>
+      <c r="H17" s="56">
+        <v>15</v>
+      </c>
+      <c r="I17" s="56">
+        <v>20</v>
+      </c>
+      <c r="J17" s="56">
+        <v>10</v>
+      </c>
+      <c r="K17" s="56">
+        <v>10</v>
+      </c>
+      <c r="L17" s="56">
+        <v>15</v>
+      </c>
+      <c r="M17" s="56">
+        <v>20</v>
+      </c>
+      <c r="N17" s="56">
+        <v>25</v>
+      </c>
+      <c r="O17" s="56">
+        <v>20</v>
+      </c>
+      <c r="P17" s="56">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="89" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" s="90" t="s">
+        <v>95</v>
+      </c>
+      <c r="L19" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="M19" s="90" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="108" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="83">
+        <v>1</v>
+      </c>
+      <c r="E20" s="93">
+        <v>3</v>
+      </c>
+      <c r="F20" s="93">
+        <v>30</v>
+      </c>
+      <c r="G20" s="93">
+        <v>2</v>
+      </c>
+      <c r="H20" s="93">
+        <v>3</v>
+      </c>
+      <c r="I20" s="93">
+        <v>2</v>
+      </c>
+      <c r="J20" s="93">
+        <v>50</v>
+      </c>
+      <c r="K20" s="93">
+        <f>F20*(E20+G20)</f>
+        <v>150</v>
+      </c>
+      <c r="L20" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="M20" s="93" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="84" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="85">
+        <v>1</v>
+      </c>
+      <c r="E21" s="93">
+        <v>2</v>
+      </c>
+      <c r="F21" s="93">
+        <v>35</v>
+      </c>
+      <c r="G21" s="93">
+        <v>1</v>
+      </c>
+      <c r="H21" s="93">
+        <v>3</v>
+      </c>
+      <c r="I21" s="93">
+        <v>2</v>
+      </c>
+      <c r="J21" s="93">
+        <v>50</v>
+      </c>
+      <c r="K21" s="93">
+        <f>F21*(E21+G21)</f>
+        <v>105</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M21" s="93" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="84" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="85">
+        <v>1</v>
+      </c>
+      <c r="E22" s="93">
+        <v>2</v>
+      </c>
+      <c r="F22" s="93">
+        <v>30</v>
+      </c>
+      <c r="G22" s="93">
+        <v>1</v>
+      </c>
+      <c r="H22" s="93">
+        <v>3</v>
+      </c>
+      <c r="I22" s="93">
+        <v>2</v>
+      </c>
+      <c r="J22" s="93">
+        <v>50</v>
+      </c>
+      <c r="K22" s="93">
+        <f>F22*(E22+G22)</f>
+        <v>90</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M22" s="93" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="85">
+        <v>1</v>
+      </c>
+      <c r="E23" s="93">
+        <v>3</v>
+      </c>
+      <c r="F23" s="93">
+        <v>35</v>
+      </c>
+      <c r="G23" s="93">
+        <v>2</v>
+      </c>
+      <c r="H23" s="93">
+        <v>3</v>
+      </c>
+      <c r="I23" s="93">
+        <v>2</v>
+      </c>
+      <c r="J23" s="93">
+        <v>50</v>
+      </c>
+      <c r="K23" s="93">
+        <f>F23*(E23+G23)</f>
+        <v>175</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" s="93" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="85">
+        <v>1</v>
+      </c>
+      <c r="E24" s="93">
+        <v>3</v>
+      </c>
+      <c r="F24" s="93">
+        <v>45</v>
+      </c>
+      <c r="G24" s="93">
+        <v>1</v>
+      </c>
+      <c r="H24" s="93">
+        <v>3</v>
+      </c>
+      <c r="I24" s="93">
+        <v>2</v>
+      </c>
+      <c r="J24" s="93">
+        <v>50</v>
+      </c>
+      <c r="K24" s="93">
+        <f>F24*(E24+G24)</f>
+        <v>180</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M24" s="93" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="97" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="84" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="109">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1">
+        <v>75</v>
+      </c>
+      <c r="G25" s="1">
+        <v>3</v>
+      </c>
+      <c r="H25" s="93">
+        <v>3</v>
+      </c>
+      <c r="I25" s="93">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1">
+        <v>100</v>
+      </c>
+      <c r="K25" s="93">
+        <f>F25*(E25+G25)</f>
+        <v>600</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="97" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="85">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>70</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4</v>
+      </c>
+      <c r="H26" s="93">
+        <v>3</v>
+      </c>
+      <c r="I26" s="93">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1">
+        <v>50</v>
+      </c>
+      <c r="K26" s="93">
+        <f>F26*(E26+G26)</f>
+        <v>560</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="85">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>4</v>
+      </c>
+      <c r="F27" s="1">
+        <v>90</v>
+      </c>
+      <c r="G27" s="1">
+        <v>3</v>
+      </c>
+      <c r="H27" s="93">
+        <v>3</v>
+      </c>
+      <c r="I27" s="93">
+        <v>2</v>
+      </c>
+      <c r="J27" s="1">
+        <v>100</v>
+      </c>
+      <c r="K27" s="93">
+        <f>F27*(E27+G27)</f>
+        <v>630</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="96" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="85">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3</v>
+      </c>
+      <c r="F28" s="1">
+        <v>80</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="93">
+        <v>3</v>
+      </c>
+      <c r="I28" s="93">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1">
+        <v>100</v>
+      </c>
+      <c r="K28" s="93">
+        <f>F28*(E28+G28)</f>
+        <v>400</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="85">
+        <v>2</v>
+      </c>
+      <c r="E29" s="93">
+        <v>6</v>
+      </c>
+      <c r="F29" s="93">
+        <v>70</v>
+      </c>
+      <c r="G29" s="93">
+        <v>3</v>
+      </c>
+      <c r="H29" s="93">
+        <v>3</v>
+      </c>
+      <c r="I29" s="93">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1">
+        <v>100</v>
+      </c>
+      <c r="K29" s="93">
+        <f>F29*(E29+G29)</f>
+        <v>630</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="97" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="85">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>150</v>
+      </c>
+      <c r="G30" s="1">
+        <v>5</v>
+      </c>
+      <c r="H30" s="93">
+        <v>3</v>
+      </c>
+      <c r="I30" s="1">
+        <v>2</v>
+      </c>
+      <c r="J30" s="1">
+        <v>200</v>
+      </c>
+      <c r="K30" s="93">
+        <f>F30*(E30+G30)</f>
+        <v>2250</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="96" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="85">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6</v>
+      </c>
+      <c r="F31" s="1">
+        <v>120</v>
+      </c>
+      <c r="G31" s="1">
+        <v>5</v>
+      </c>
+      <c r="H31" s="93">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1">
+        <v>2</v>
+      </c>
+      <c r="J31" s="1">
+        <v>200</v>
+      </c>
+      <c r="K31" s="93">
+        <f>F31*(E31+G31)</f>
+        <v>1320</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="85">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>9</v>
+      </c>
+      <c r="F32" s="1">
+        <v>80</v>
+      </c>
+      <c r="G32" s="1">
+        <v>6</v>
+      </c>
+      <c r="H32" s="93">
+        <v>3</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1">
+        <v>200</v>
+      </c>
+      <c r="K32" s="93">
+        <f>F32*(E32+G32)</f>
+        <v>1200</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="85">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>9</v>
+      </c>
+      <c r="F33" s="1">
+        <v>110</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+      <c r="H33" s="93">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1">
+        <v>2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>200</v>
+      </c>
+      <c r="K33" s="93">
+        <f>F33*(E33+G33)</f>
+        <v>1540</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="85">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1">
+        <v>100</v>
+      </c>
+      <c r="G34" s="1">
+        <v>5</v>
+      </c>
+      <c r="H34" s="93">
+        <v>3</v>
+      </c>
+      <c r="I34" s="1">
+        <v>2</v>
+      </c>
+      <c r="J34" s="1">
+        <v>200</v>
+      </c>
+      <c r="K34" s="93">
+        <f>F34*(E34+G34)</f>
+        <v>1600</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="89" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="J36" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="K36" s="90" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="111">
+        <v>1</v>
+      </c>
+      <c r="E37" s="93">
+        <v>3</v>
+      </c>
+      <c r="F37" s="93">
+        <v>35</v>
+      </c>
+      <c r="G37" s="93">
+        <v>1</v>
+      </c>
+      <c r="H37" s="93">
+        <v>3</v>
+      </c>
+      <c r="I37" s="93">
+        <v>2</v>
+      </c>
+      <c r="J37" s="93">
+        <v>50</v>
+      </c>
+      <c r="K37" s="93">
+        <f>F37*(E37+G37)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D38" s="85">
+        <v>2</v>
+      </c>
+      <c r="E38" s="93">
+        <v>5</v>
+      </c>
+      <c r="F38" s="93">
+        <v>70</v>
+      </c>
+      <c r="G38" s="93">
+        <v>3</v>
+      </c>
+      <c r="H38" s="93">
+        <v>3</v>
+      </c>
+      <c r="I38" s="93">
+        <v>2</v>
+      </c>
+      <c r="J38" s="1">
+        <v>100</v>
+      </c>
+      <c r="K38" s="93">
+        <f>F38*(E38+G38)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D39" s="85">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1">
+        <v>100</v>
+      </c>
+      <c r="G39" s="1">
+        <v>5</v>
+      </c>
+      <c r="H39" s="93">
+        <v>3</v>
+      </c>
+      <c r="I39" s="1">
+        <v>2</v>
+      </c>
+      <c r="J39" s="1">
+        <v>200</v>
+      </c>
+      <c r="K39" s="93">
+        <f>F39*(E39+G39)</f>
+        <v>1500</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A19:M34">
+    <sortState ref="A20:M34">
+      <sortCondition ref="D19:D34"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="R3:R14">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:F15">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P15">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q15">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D24 D26:D34">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:Q17">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:Q15">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="33" id="{CFA98A31-3F14-4BF5-85DA-33E0BA96141A}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D20:D24 D26:D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="15" id="{7E3A0E15-F45D-440D-AED9-3247B2F81BF5}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="14" id="{8280124A-7690-41C0-84FD-7DB9F7E5356B}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D20:D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="12" id="{6EE9C0AD-70C1-42CC-BB38-155FC27ECDAE}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D37</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{E60CCE82-C16F-46E7-B840-B62D165E4FFC}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D38</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{9A93E340-B874-431B-92AA-3B545E97243E}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D39</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
GDD paar kapiteln rein Level up glory stufen definiert
</commit_message>
<xml_diff>
--- a/Game Design/BL_Map_Tiles.xlsx
+++ b/Game Design/BL_Map_Tiles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="49665" yWindow="75" windowWidth="16860" windowHeight="6255" activeTab="3"/>
+    <workbookView xWindow="49665" yWindow="75" windowWidth="16860" windowHeight="6255" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="terrain" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="119">
   <si>
     <t>Temperature</t>
   </si>
@@ -222,18 +222,6 @@
     <t>lvl</t>
   </si>
   <si>
-    <t>enemy</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>***</t>
-  </si>
-  <si>
     <t>aw</t>
   </si>
   <si>
@@ -345,9 +333,6 @@
     <t>def</t>
   </si>
   <si>
-    <t>exp</t>
-  </si>
-  <si>
     <t>glory</t>
   </si>
   <si>
@@ -430,6 +415,9 @@
   </si>
   <si>
     <t>MUSTER</t>
+  </si>
+  <si>
+    <t>*3</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1290,27 +1278,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1372,13 +1339,52 @@
     <xf numFmtId="9" fontId="2" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1684,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:R20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,43 +1714,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="76" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="76" t="s">
+      <c r="E1" s="108"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="75" t="s">
+      <c r="N1" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="80"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="111"/>
       <c r="R1" s="48" t="s">
         <v>31</v>
       </c>
       <c r="S1" s="52"/>
       <c r="T1" s="1"/>
-      <c r="U1" s="74" t="s">
+      <c r="U1" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
+      <c r="V1" s="106"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="106"/>
+      <c r="Y1" s="106"/>
+      <c r="Z1" s="106"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1774,7 +1780,7 @@
       <c r="I2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="79"/>
+      <c r="J2" s="110"/>
       <c r="N2" s="39" t="s">
         <v>25</v>
       </c>
@@ -1793,7 +1799,7 @@
       <c r="S2" s="52"/>
       <c r="T2" s="1"/>
       <c r="V2" s="39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="W2" s="39" t="s">
         <v>35</v>
@@ -2654,7 +2660,7 @@
         <v>24</v>
       </c>
       <c r="Q16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -3021,7 +3027,7 @@
     <row r="3" spans="3:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="73" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>40</v>
@@ -3119,17 +3125,17 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3139,196 +3145,430 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="116" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="116" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="116" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="116" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="116" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="117" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="118">
         <v>1</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="1">
         <f>B3-B2</f>
+        <v>400</v>
+      </c>
+      <c r="D2" s="1">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="114">
+        <v>3</v>
+      </c>
+      <c r="H2" s="115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="118">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>400</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C5" si="0">B4-B3</f>
+        <v>1100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="114">
+        <v>3</v>
+      </c>
+      <c r="H3" s="115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="118">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="D4" s="1">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="114">
+        <v>3</v>
+      </c>
+      <c r="H4" s="115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="118">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="D5" s="1">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8</v>
+      </c>
+      <c r="G5" s="114">
+        <v>3</v>
+      </c>
+      <c r="H5" s="115">
+        <v>2</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="118">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10</v>
+      </c>
+      <c r="G6" s="114">
+        <v>3</v>
+      </c>
+      <c r="H6" s="115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="112" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="112" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="103">
+        <v>1</v>
+      </c>
+      <c r="C11" s="86">
+        <v>3</v>
+      </c>
+      <c r="D11" s="86">
+        <v>35</v>
+      </c>
+      <c r="E11" s="86">
+        <v>1</v>
+      </c>
+      <c r="F11" s="113">
+        <v>3</v>
+      </c>
+      <c r="G11" s="113">
+        <v>2</v>
+      </c>
+      <c r="H11" s="86">
+        <f>D11*(C11+E11)</f>
+        <v>140</v>
+      </c>
+      <c r="I11">
+        <f>H11*3</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="78">
+        <v>2</v>
+      </c>
+      <c r="C12" s="86">
+        <v>5</v>
+      </c>
+      <c r="D12" s="86">
+        <v>70</v>
+      </c>
+      <c r="E12" s="86">
+        <v>3</v>
+      </c>
+      <c r="F12" s="113">
+        <v>3</v>
+      </c>
+      <c r="G12" s="113">
+        <v>2</v>
+      </c>
+      <c r="H12" s="86">
+        <f>D12*(C12+E12)</f>
+        <v>560</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I13" si="1">H12*3</f>
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="78">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
         <v>100</v>
       </c>
-      <c r="D2" s="26">
-        <v>20</v>
-      </c>
-      <c r="E2" s="26">
-        <v>6</v>
-      </c>
-      <c r="F2" s="26">
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" s="113">
+        <v>3</v>
+      </c>
+      <c r="G13" s="114">
         <v>2</v>
       </c>
-      <c r="G2" s="26">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
-        <v>2</v>
-      </c>
-      <c r="B3" s="26">
-        <v>100</v>
-      </c>
-      <c r="C3" s="26">
-        <f t="shared" ref="C3:C5" si="0">B4-B3</f>
-        <v>400</v>
-      </c>
-      <c r="D3" s="26">
-        <v>25</v>
-      </c>
-      <c r="E3" s="26">
-        <v>9</v>
-      </c>
-      <c r="F3" s="26">
-        <v>4</v>
-      </c>
-      <c r="G3" s="26">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
-        <v>3</v>
-      </c>
-      <c r="B4" s="26">
-        <v>500</v>
-      </c>
-      <c r="C4" s="26">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="D4" s="26">
-        <v>30</v>
-      </c>
-      <c r="E4" s="26">
-        <v>11</v>
-      </c>
-      <c r="F4" s="26">
-        <v>6</v>
-      </c>
-      <c r="G4" s="26">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
-        <v>4</v>
-      </c>
-      <c r="B5" s="26">
-        <v>1300</v>
-      </c>
-      <c r="C5" s="26">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="D5" s="26">
-        <v>35</v>
-      </c>
-      <c r="E5" s="26">
-        <v>14</v>
-      </c>
-      <c r="F5" s="26">
-        <v>8</v>
-      </c>
-      <c r="G5" s="26">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="K5" s="26">
-        <v>50</v>
-      </c>
-      <c r="L5" s="26">
-        <v>100</v>
-      </c>
-      <c r="M5" s="26">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
-        <v>5</v>
-      </c>
-      <c r="B6" s="26">
-        <v>2500</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26">
-        <v>40</v>
-      </c>
-      <c r="E6" s="26">
-        <v>17</v>
-      </c>
-      <c r="F6" s="26">
-        <v>10</v>
-      </c>
-      <c r="G6" s="26">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
+      <c r="H13" s="86">
+        <f>D13*(C13+E13)</f>
+        <v>1500</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>4500</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H6"/>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="12" id="{01DDC6C4-AC6B-42AE-91BA-4DB5D91358B6}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{20239F9C-485D-479C-A879-E90CFCBEEE47}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{623A8F77-A078-4188-A6E6-654FB1360156}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B13</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3336,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3354,79 +3594,79 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="26"/>
-      <c r="C1" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
+      <c r="C1" s="106" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
       <c r="R1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="110"/>
+      <c r="S1" s="102"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="H2" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="I2" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="J2" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="K2" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="L2" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="M2" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="N2" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="O2" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="L2" s="84" t="s">
+      <c r="P2" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="84" t="s">
+      <c r="Q2" s="77" t="s">
         <v>81</v>
-      </c>
-      <c r="N2" s="84" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" s="84" t="s">
-        <v>83</v>
-      </c>
-      <c r="P2" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q2" s="84" t="s">
-        <v>85</v>
       </c>
       <c r="R2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="110"/>
+      <c r="S2" s="102"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -3435,34 +3675,34 @@
       <c r="B3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="L3" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="M3" s="102"/>
-      <c r="N3" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="102"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="L3" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="M3" s="95"/>
+      <c r="N3" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
       <c r="R3" s="50">
         <f>SUM(C3:Q3)</f>
         <v>0.2</v>
       </c>
-      <c r="S3" s="110"/>
+      <c r="S3" s="102"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -3471,34 +3711,34 @@
       <c r="B4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="L4" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="M4" s="102"/>
-      <c r="N4" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="L4" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="M4" s="95"/>
+      <c r="N4" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
       <c r="R4" s="50">
         <f t="shared" ref="R4:R14" si="0">SUM(C4:Q4)</f>
         <v>0.2</v>
       </c>
-      <c r="S4" s="110"/>
+      <c r="S4" s="102"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -3507,34 +3747,34 @@
       <c r="B5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="L5" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="M5" s="102"/>
-      <c r="N5" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="O5" s="102"/>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="L5" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="95"/>
+      <c r="N5" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
       <c r="R5" s="50">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="S5" s="110"/>
+      <c r="S5" s="102"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -3543,34 +3783,34 @@
       <c r="B6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="H6" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="102"/>
-      <c r="N6" s="102"/>
-      <c r="O6" s="102"/>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="101">
+      <c r="C6" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="94">
         <v>0.05</v>
       </c>
       <c r="R6" s="50">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="S6" s="110"/>
+      <c r="S6" s="102"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -3579,32 +3819,32 @@
       <c r="B7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="N7" s="102"/>
-      <c r="O7" s="102"/>
-      <c r="P7" s="102"/>
-      <c r="Q7" s="101">
+      <c r="C7" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="N7" s="95"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="94">
         <v>0.05</v>
       </c>
       <c r="R7" s="50">
         <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="S7" s="110"/>
+      <c r="S7" s="102"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -3613,34 +3853,34 @@
       <c r="B8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="M8" s="102"/>
-      <c r="N8" s="102"/>
-      <c r="O8" s="102"/>
-      <c r="P8" s="102"/>
-      <c r="Q8" s="101">
+      <c r="C8" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="95"/>
+      <c r="G8" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="95"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="M8" s="95"/>
+      <c r="N8" s="95"/>
+      <c r="O8" s="95"/>
+      <c r="P8" s="95"/>
+      <c r="Q8" s="94">
         <v>0.05</v>
       </c>
       <c r="R8" s="50">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="S8" s="110"/>
+      <c r="S8" s="102"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -3649,32 +3889,32 @@
       <c r="B9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="Q9" s="102"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="K9" s="95"/>
+      <c r="L9" s="95"/>
+      <c r="M9" s="95"/>
+      <c r="N9" s="95"/>
+      <c r="O9" s="95"/>
+      <c r="P9" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="Q9" s="95"/>
       <c r="R9" s="50">
         <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="S9" s="110"/>
+      <c r="S9" s="102"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -3683,34 +3923,34 @@
       <c r="B10" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="N10" s="102"/>
-      <c r="O10" s="102"/>
-      <c r="P10" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="Q10" s="102"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="K10" s="95"/>
+      <c r="L10" s="95"/>
+      <c r="M10" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="N10" s="95"/>
+      <c r="O10" s="95"/>
+      <c r="P10" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="Q10" s="95"/>
       <c r="R10" s="50">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="S10" s="110"/>
+      <c r="S10" s="102"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -3719,36 +3959,36 @@
       <c r="B11" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="K11" s="102"/>
-      <c r="L11" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="M11" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="N11" s="102"/>
-      <c r="O11" s="102"/>
-      <c r="P11" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="Q11" s="102"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="95"/>
+      <c r="I11" s="95"/>
+      <c r="J11" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="K11" s="95"/>
+      <c r="L11" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="M11" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="N11" s="95"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="Q11" s="95"/>
       <c r="R11" s="50">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="S11" s="110"/>
+      <c r="S11" s="102"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -3757,32 +3997,32 @@
       <c r="B12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="D12" s="100"/>
-      <c r="E12" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="102"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="102"/>
-      <c r="O12" s="102"/>
-      <c r="P12" s="102"/>
-      <c r="Q12" s="101">
+      <c r="C12" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="93"/>
+      <c r="E12" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="95"/>
+      <c r="N12" s="95"/>
+      <c r="O12" s="95"/>
+      <c r="P12" s="95"/>
+      <c r="Q12" s="94">
         <v>0.05</v>
       </c>
       <c r="R12" s="50">
         <f t="shared" si="0"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="S12" s="110"/>
+      <c r="S12" s="102"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -3791,34 +4031,34 @@
       <c r="B13" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="103">
-        <v>0.05</v>
-      </c>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="H13" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="101">
+      <c r="C13" s="96">
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="H13" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="I13" s="95"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="95"/>
+      <c r="N13" s="95"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="94">
         <v>0.05</v>
       </c>
       <c r="R13" s="50">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="S13" s="110"/>
+      <c r="S13" s="102"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -3827,95 +4067,95 @@
       <c r="B14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="104"/>
-      <c r="D14" s="105">
-        <v>0.05</v>
-      </c>
-      <c r="E14" s="104"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="107">
-        <v>0.05</v>
-      </c>
-      <c r="I14" s="107">
-        <v>0.05</v>
-      </c>
-      <c r="J14" s="106"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="106"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="106"/>
-      <c r="O14" s="107">
-        <v>0.05</v>
-      </c>
-      <c r="P14" s="106"/>
-      <c r="Q14" s="106"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="98">
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="97"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="100">
+        <v>0.05</v>
+      </c>
+      <c r="I14" s="100">
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="100">
+        <v>0.05</v>
+      </c>
+      <c r="P14" s="99"/>
+      <c r="Q14" s="99"/>
       <c r="R14" s="50">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="S14" s="110"/>
+      <c r="S14" s="102"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26"/>
       <c r="C15" s="44">
-        <f>SUM(C3:C14)</f>
+        <f t="shared" ref="C15:Q15" si="1">SUM(C3:C14)</f>
         <v>0.25</v>
       </c>
       <c r="D15" s="45">
-        <f>SUM(D3:D14)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="E15" s="45">
-        <f>SUM(E3:E14)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F15" s="46">
-        <f>SUM(F3:F14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="G15" s="46">
-        <f>SUM(G3:G14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="H15" s="46">
-        <f>SUM(H3:H14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="I15" s="46">
-        <f>SUM(I3:I14)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="J15" s="46">
-        <f>SUM(J3:J14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="K15" s="46">
-        <f>SUM(K3:K14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="L15" s="46">
-        <f>SUM(L3:L14)</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="M15" s="46">
-        <f>SUM(M3:M14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="N15" s="46">
-        <f>SUM(N3:N14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="O15" s="46">
-        <f>SUM(O3:O14)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="P15" s="46">
-        <f>SUM(P3:P14)</f>
+        <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="Q15" s="46">
-        <f>SUM(Q3:Q14)</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="R15" s="41"/>
@@ -3977,308 +4217,294 @@
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="79" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="86" t="s">
+      <c r="F19" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="86" t="s">
+      <c r="H19" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="I19" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="87" t="s">
+      <c r="J19" s="82"/>
+      <c r="K19" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="88" t="s">
+      <c r="L19" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="89" t="s">
+      <c r="M19" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="89" t="s">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="104" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="76">
+        <v>1</v>
+      </c>
+      <c r="E20" s="86">
+        <v>2</v>
+      </c>
+      <c r="F20" s="86">
+        <v>30</v>
+      </c>
+      <c r="G20" s="86">
+        <v>1</v>
+      </c>
+      <c r="H20" s="86">
+        <v>3</v>
+      </c>
+      <c r="I20" s="86">
+        <v>2</v>
+      </c>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86">
+        <f t="shared" ref="K20:K34" si="2">F20*(E20+G20)</f>
+        <v>90</v>
+      </c>
+      <c r="L20" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="M20" s="86" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="J19" s="89" t="s">
+      <c r="B21" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="78">
+        <v>1</v>
+      </c>
+      <c r="E21" s="86">
+        <v>2</v>
+      </c>
+      <c r="F21" s="86">
+        <v>35</v>
+      </c>
+      <c r="G21" s="86">
+        <v>1</v>
+      </c>
+      <c r="H21" s="86">
+        <v>3</v>
+      </c>
+      <c r="I21" s="86">
+        <v>2</v>
+      </c>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K19" s="90" t="s">
+      <c r="M21" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="L19" s="91" t="s">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="78">
+        <v>1</v>
+      </c>
+      <c r="E22" s="86">
+        <v>3</v>
+      </c>
+      <c r="F22" s="86">
+        <v>30</v>
+      </c>
+      <c r="G22" s="86">
+        <v>2</v>
+      </c>
+      <c r="H22" s="86">
+        <v>3</v>
+      </c>
+      <c r="I22" s="86">
+        <v>2</v>
+      </c>
+      <c r="J22" s="86"/>
+      <c r="K22" s="86">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M22" s="86" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="78">
+        <v>1</v>
+      </c>
+      <c r="E23" s="86">
+        <v>3</v>
+      </c>
+      <c r="F23" s="86">
+        <v>35</v>
+      </c>
+      <c r="G23" s="86">
+        <v>2</v>
+      </c>
+      <c r="H23" s="86">
+        <v>3</v>
+      </c>
+      <c r="I23" s="86">
+        <v>2</v>
+      </c>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M23" s="86" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="M19" s="90" t="s">
+      <c r="B24" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="78">
+        <v>1</v>
+      </c>
+      <c r="E24" s="86">
+        <v>3</v>
+      </c>
+      <c r="F24" s="86">
+        <v>45</v>
+      </c>
+      <c r="G24" s="86">
+        <v>1</v>
+      </c>
+      <c r="H24" s="86">
+        <v>3</v>
+      </c>
+      <c r="I24" s="86">
+        <v>2</v>
+      </c>
+      <c r="J24" s="86"/>
+      <c r="K24" s="86">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="M24" s="86" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="78">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>80</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="86">
+        <v>3</v>
+      </c>
+      <c r="I25" s="86">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="86">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="88" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="92" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="83">
-        <v>1</v>
-      </c>
-      <c r="E20" s="93">
-        <v>3</v>
-      </c>
-      <c r="F20" s="93">
-        <v>30</v>
-      </c>
-      <c r="G20" s="93">
-        <v>2</v>
-      </c>
-      <c r="H20" s="93">
-        <v>3</v>
-      </c>
-      <c r="I20" s="93">
-        <v>2</v>
-      </c>
-      <c r="J20" s="93">
-        <v>50</v>
-      </c>
-      <c r="K20" s="93">
-        <f>F20*(E20+G20)</f>
-        <v>150</v>
-      </c>
-      <c r="L20" s="93" t="s">
-        <v>106</v>
-      </c>
-      <c r="M20" s="93" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="98" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="84" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="85">
-        <v>1</v>
-      </c>
-      <c r="E21" s="93">
-        <v>2</v>
-      </c>
-      <c r="F21" s="93">
-        <v>35</v>
-      </c>
-      <c r="G21" s="93">
-        <v>1</v>
-      </c>
-      <c r="H21" s="93">
-        <v>3</v>
-      </c>
-      <c r="I21" s="93">
-        <v>2</v>
-      </c>
-      <c r="J21" s="93">
-        <v>50</v>
-      </c>
-      <c r="K21" s="93">
-        <f>F21*(E21+G21)</f>
-        <v>105</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M21" s="93" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="96" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="84" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="85">
-        <v>1</v>
-      </c>
-      <c r="E22" s="93">
-        <v>2</v>
-      </c>
-      <c r="F22" s="93">
-        <v>30</v>
-      </c>
-      <c r="G22" s="93">
-        <v>1</v>
-      </c>
-      <c r="H22" s="93">
-        <v>3</v>
-      </c>
-      <c r="I22" s="93">
-        <v>2</v>
-      </c>
-      <c r="J22" s="93">
-        <v>50</v>
-      </c>
-      <c r="K22" s="93">
-        <f>F22*(E22+G22)</f>
-        <v>90</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M22" s="93" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="96" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="95" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="85">
-        <v>1</v>
-      </c>
-      <c r="E23" s="93">
-        <v>3</v>
-      </c>
-      <c r="F23" s="93">
-        <v>35</v>
-      </c>
-      <c r="G23" s="93">
-        <v>2</v>
-      </c>
-      <c r="H23" s="93">
-        <v>3</v>
-      </c>
-      <c r="I23" s="93">
-        <v>2</v>
-      </c>
-      <c r="J23" s="93">
-        <v>50</v>
-      </c>
-      <c r="K23" s="93">
-        <f>F23*(E23+G23)</f>
-        <v>175</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="M23" s="93" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="84" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="85">
-        <v>1</v>
-      </c>
-      <c r="E24" s="93">
-        <v>3</v>
-      </c>
-      <c r="F24" s="93">
-        <v>45</v>
-      </c>
-      <c r="G24" s="93">
-        <v>1</v>
-      </c>
-      <c r="H24" s="93">
-        <v>3</v>
-      </c>
-      <c r="I24" s="93">
-        <v>2</v>
-      </c>
-      <c r="J24" s="93">
-        <v>50</v>
-      </c>
-      <c r="K24" s="93">
-        <f>F24*(E24+G24)</f>
-        <v>180</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M24" s="93" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="97" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="109">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1">
-        <v>5</v>
-      </c>
-      <c r="F25" s="1">
-        <v>75</v>
-      </c>
-      <c r="G25" s="1">
-        <v>3</v>
-      </c>
-      <c r="H25" s="93">
-        <v>3</v>
-      </c>
-      <c r="I25" s="93">
-        <v>2</v>
-      </c>
-      <c r="J25" s="1">
-        <v>100</v>
-      </c>
-      <c r="K25" s="93">
-        <f>F25*(E25+G25)</f>
-        <v>600</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="97" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" s="95" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="85">
+      <c r="C26" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="78">
         <v>2</v>
       </c>
       <c r="E26" s="1">
@@ -4290,205 +4516,195 @@
       <c r="G26" s="1">
         <v>4</v>
       </c>
-      <c r="H26" s="93">
+      <c r="H26" s="86">
         <v>3</v>
       </c>
-      <c r="I26" s="93">
+      <c r="I26" s="86">
         <v>2</v>
       </c>
-      <c r="J26" s="1">
-        <v>50</v>
-      </c>
-      <c r="K26" s="93">
-        <f>F26*(E26+G26)</f>
+      <c r="J26" s="1"/>
+      <c r="K26" s="86">
+        <f t="shared" si="2"/>
         <v>560</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="98" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="85">
+      <c r="A27" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="101">
         <v>2</v>
       </c>
       <c r="E27" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" s="1">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="G27" s="1">
         <v>3</v>
       </c>
-      <c r="H27" s="93">
+      <c r="H27" s="86">
         <v>3</v>
       </c>
-      <c r="I27" s="93">
+      <c r="I27" s="86">
         <v>2</v>
       </c>
-      <c r="J27" s="1">
-        <v>100</v>
-      </c>
-      <c r="K27" s="93">
-        <f>F27*(E27+G27)</f>
+      <c r="J27" s="1"/>
+      <c r="K27" s="86">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="78">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1">
+        <v>90</v>
+      </c>
+      <c r="G28" s="1">
+        <v>3</v>
+      </c>
+      <c r="H28" s="86">
+        <v>3</v>
+      </c>
+      <c r="I28" s="86">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="86">
+        <f t="shared" si="2"/>
         <v>630</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="96" t="s">
-        <v>120</v>
-      </c>
-      <c r="B28" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="85">
+      <c r="L28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="92" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="78">
         <v>2</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E29" s="86">
+        <v>6</v>
+      </c>
+      <c r="F29" s="86">
+        <v>70</v>
+      </c>
+      <c r="G29" s="86">
         <v>3</v>
       </c>
-      <c r="F28" s="1">
+      <c r="H29" s="86">
+        <v>3</v>
+      </c>
+      <c r="I29" s="86">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="86">
+        <f t="shared" si="2"/>
+        <v>630</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="78">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1">
         <v>80</v>
       </c>
-      <c r="G28" s="1">
-        <v>2</v>
-      </c>
-      <c r="H28" s="93">
-        <v>3</v>
-      </c>
-      <c r="I28" s="93">
-        <v>2</v>
-      </c>
-      <c r="J28" s="1">
-        <v>100</v>
-      </c>
-      <c r="K28" s="93">
-        <f>F28*(E28+G28)</f>
-        <v>400</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="99" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="84" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="85">
-        <v>2</v>
-      </c>
-      <c r="E29" s="93">
+      <c r="G30" s="1">
         <v>6</v>
       </c>
-      <c r="F29" s="93">
-        <v>70</v>
-      </c>
-      <c r="G29" s="93">
-        <v>3</v>
-      </c>
-      <c r="H29" s="93">
-        <v>3</v>
-      </c>
-      <c r="I29" s="93">
-        <v>2</v>
-      </c>
-      <c r="J29" s="1">
-        <v>100</v>
-      </c>
-      <c r="K29" s="93">
-        <f>F29*(E29+G29)</f>
-        <v>630</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="97" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="84" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="85">
-        <v>3</v>
-      </c>
-      <c r="E30" s="1">
-        <v>10</v>
-      </c>
-      <c r="F30" s="1">
-        <v>150</v>
-      </c>
-      <c r="G30" s="1">
-        <v>5</v>
-      </c>
-      <c r="H30" s="93">
+      <c r="H30" s="86">
         <v>3</v>
       </c>
       <c r="I30" s="1">
         <v>2</v>
       </c>
-      <c r="J30" s="1">
-        <v>200</v>
-      </c>
-      <c r="K30" s="93">
-        <f>F30*(E30+G30)</f>
-        <v>2250</v>
+      <c r="J30" s="1"/>
+      <c r="K30" s="86">
+        <f t="shared" si="2"/>
+        <v>1200</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>106</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="96" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="84" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="85">
+      <c r="A31" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="78">
         <v>3</v>
       </c>
       <c r="E31" s="1">
@@ -4500,238 +4716,221 @@
       <c r="G31" s="1">
         <v>5</v>
       </c>
-      <c r="H31" s="93">
+      <c r="H31" s="86">
         <v>3</v>
       </c>
       <c r="I31" s="1">
         <v>2</v>
       </c>
-      <c r="J31" s="1">
-        <v>200</v>
-      </c>
-      <c r="K31" s="93">
-        <f>F31*(E31+G31)</f>
+      <c r="J31" s="1"/>
+      <c r="K31" s="86">
+        <f t="shared" si="2"/>
         <v>1320</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="94" t="s">
-        <v>101</v>
-      </c>
-      <c r="B32" s="95" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="84" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="85">
+      <c r="A32" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="78">
         <v>3</v>
       </c>
       <c r="E32" s="1">
         <v>9</v>
       </c>
       <c r="F32" s="1">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="G32" s="1">
-        <v>6</v>
-      </c>
-      <c r="H32" s="93">
+        <v>5</v>
+      </c>
+      <c r="H32" s="86">
         <v>3</v>
       </c>
       <c r="I32" s="1">
         <v>2</v>
       </c>
-      <c r="J32" s="1">
-        <v>200</v>
-      </c>
-      <c r="K32" s="93">
-        <f>F32*(E32+G32)</f>
-        <v>1200</v>
+      <c r="J32" s="1"/>
+      <c r="K32" s="86">
+        <f t="shared" si="2"/>
+        <v>1540</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="94" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="84" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="85">
+      <c r="A33" s="91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="78">
         <v>3</v>
       </c>
       <c r="E33" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F33" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G33" s="1">
         <v>5</v>
       </c>
-      <c r="H33" s="93">
+      <c r="H33" s="86">
         <v>3</v>
       </c>
       <c r="I33" s="1">
         <v>2</v>
       </c>
-      <c r="J33" s="1">
-        <v>200</v>
-      </c>
-      <c r="K33" s="93">
-        <f>F33*(E33+G33)</f>
-        <v>1540</v>
+      <c r="J33" s="1"/>
+      <c r="K33" s="86">
+        <f t="shared" si="2"/>
+        <v>1600</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="98" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="85">
+      <c r="A34" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="78">
         <v>3</v>
       </c>
       <c r="E34" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G34" s="1">
         <v>5</v>
       </c>
-      <c r="H34" s="93">
+      <c r="H34" s="86">
         <v>3</v>
       </c>
       <c r="I34" s="1">
         <v>2</v>
       </c>
-      <c r="J34" s="1">
-        <v>200</v>
-      </c>
-      <c r="K34" s="93">
-        <f>F34*(E34+G34)</f>
-        <v>1600</v>
+      <c r="J34" s="1"/>
+      <c r="K34" s="86">
+        <f t="shared" si="2"/>
+        <v>2250</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="87" t="s">
+      <c r="D36" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="G36" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36" s="82" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="J36" s="83" t="s">
         <v>90</v>
-      </c>
-      <c r="F36" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="89" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J36" s="89" t="s">
-        <v>94</v>
-      </c>
-      <c r="K36" s="90" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="63" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" s="111">
+        <v>117</v>
+      </c>
+      <c r="D37" s="103">
         <v>1</v>
       </c>
-      <c r="E37" s="93">
+      <c r="E37" s="86">
         <v>3</v>
       </c>
-      <c r="F37" s="93">
+      <c r="F37" s="86">
         <v>35</v>
       </c>
-      <c r="G37" s="93">
+      <c r="G37" s="86">
         <v>1</v>
       </c>
-      <c r="H37" s="93">
+      <c r="H37" s="86">
         <v>3</v>
       </c>
-      <c r="I37" s="93">
+      <c r="I37" s="86">
         <v>2</v>
       </c>
-      <c r="J37" s="93">
-        <v>50</v>
-      </c>
-      <c r="K37" s="93">
+      <c r="J37" s="86">
         <f>F37*(E37+G37)</f>
         <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D38" s="85">
+      <c r="D38" s="78">
         <v>2</v>
       </c>
-      <c r="E38" s="93">
+      <c r="E38" s="86">
         <v>5</v>
       </c>
-      <c r="F38" s="93">
+      <c r="F38" s="86">
         <v>70</v>
       </c>
-      <c r="G38" s="93">
+      <c r="G38" s="86">
         <v>3</v>
       </c>
-      <c r="H38" s="93">
+      <c r="H38" s="86">
         <v>3</v>
       </c>
-      <c r="I38" s="93">
+      <c r="I38" s="86">
         <v>2</v>
       </c>
-      <c r="J38" s="1">
-        <v>100</v>
-      </c>
-      <c r="K38" s="93">
+      <c r="J38" s="86">
         <f>F38*(E38+G38)</f>
         <v>560</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D39" s="85">
+      <c r="D39" s="78">
         <v>3</v>
       </c>
       <c r="E39" s="1">
@@ -4743,16 +4942,13 @@
       <c r="G39" s="1">
         <v>5</v>
       </c>
-      <c r="H39" s="93">
+      <c r="H39" s="86">
         <v>3</v>
       </c>
       <c r="I39" s="1">
         <v>2</v>
       </c>
-      <c r="J39" s="1">
-        <v>200</v>
-      </c>
-      <c r="K39" s="93">
+      <c r="J39" s="86">
         <f>F39*(E39+G39)</f>
         <v>1500</v>
       </c>
@@ -4760,7 +4956,7 @@
   </sheetData>
   <autoFilter ref="A19:M34">
     <sortState ref="A20:M34">
-      <sortCondition ref="D19:D34"/>
+      <sortCondition ref="K19:K34"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">

</xml_diff>